<commit_message>
changes structure of resources folder
</commit_message>
<xml_diff>
--- a/resources/Customer/Customer.xlsx
+++ b/resources/Customer/Customer.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56E3992-7F5B-4089-B3F5-55F11AFC2F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB99903-593B-4BE0-B6C3-1C375F2FF52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7065" yWindow="1770" windowWidth="12825" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -163,15 +163,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -179,17 +191,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -532,7 +561,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C11" sqref="C11:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,180 +573,181 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="B11" s="4"/>
       <c r="C11" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="4">
         <v>1032547698</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="4">
         <v>10000</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>